<commit_message>
Moved AN220 scripts to their output folders
</commit_message>
<xml_diff>
--- a/src/Pickles/MIL_pickles/Output/AN220/AN220_TestScript_Desktop_Admin_System_FR_NFR.xlsx
+++ b/src/Pickles/MIL_pickles/Output/AN220/AN220_TestScript_Desktop_Admin_System_FR_NFR.xlsx
@@ -36,7 +36,7 @@
     <x:t>Tags:</x:t>
   </x:si>
   <x:si>
-    <x:t>@FR, @FR031, @UR029, @Admin, @DesktopOnly</x:t>
+    <x:t>@FR, @FR031, @UR029, @Admin, @DesktopOnly, @deprecated</x:t>
   </x:si>
   <x:si>
     <x:t>CannotRegisterInCECountry</x:t>
@@ -81,7 +81,7 @@
     <x:t>CustomerWorkflowUK</x:t>
   </x:si>
   <x:si>
-    <x:t>@FR, @FR030, @UR028, @Admin, @DesktopOnly</x:t>
+    <x:t>@FR, @FR030, @UR028, @Admin, @DesktopOnly, @deprecated</x:t>
   </x:si>
   <x:si>
     <x:t>ShowRegistrationForm</x:t>
@@ -195,7 +195,7 @@
     <x:t>DesktopLicensing</x:t>
   </x:si>
   <x:si>
-    <x:t>@FR, @FR027, @UR025, @Admin, @DesktopOnly</x:t>
+    <x:t>@FR, @FR027, @UR025, @Admin, @DesktopOnly, @deprecated</x:t>
   </x:si>
   <x:si>
     <x:t>CannotRegisterInNonCECountry</x:t>
@@ -606,7 +606,7 @@
     <x:t>DontOpenMultipleImages</x:t>
   </x:si>
   <x:si>
-    <x:t>@FR035-03, @UR033-01</x:t>
+    <x:t>@FR035-03, @UR033-01, @deprecated</x:t>
   </x:si>
   <x:si>
     <x:t>I have multiple image files</x:t>
@@ -762,7 +762,7 @@
     <x:t>LoginDisabled</x:t>
   </x:si>
   <x:si>
-    <x:t>@FR043-02, @UR041-01</x:t>
+    <x:t>@FR043-02, @UR041-01, @deprecated</x:t>
   </x:si>
   <x:si>
     <x:t>user account licensing is disabled on the store app</x:t>
@@ -975,10 +975,10 @@
     <x:t>I am logged in as a site administrator</x:t>
   </x:si>
   <x:si>
-    <x:t>I veiw the user roles</x:t>
-  </x:si>
-  <x:si>
-    <x:t>thrre is a subscriber role for users that have registered but not setup an account</x:t>
+    <x:t>I view the user roles</x:t>
+  </x:si>
+  <x:si>
+    <x:t>there is a subscriber role for users that have registered but not setup an account</x:t>
   </x:si>
   <x:si>
     <x:t>there is a Collaborator role for registered AssistDent users</x:t>
@@ -1041,7 +1041,7 @@
     <x:t>I have admin rights</x:t>
   </x:si>
   <x:si>
-    <x:t>I have created a CD Admin or CDV User</x:t>
+    <x:t>I have created a CD Admin or CD User</x:t>
   </x:si>
   <x:si>
     <x:t>I delete the user on the website</x:t>
@@ -4295,7 +4295,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D69"/>
+  <x:dimension ref="A1:D66"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -4421,226 +4421,244 @@
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4"/>
+    <x:row r="24" spans="1:4">
+      <x:c r="C24" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>249</x:v>
+      </x:c>
+    </x:row>
     <x:row r="25" spans="1:4">
-      <x:c r="B25" s="1" t="s">
-        <x:v>238</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:4"/>
-    <x:row r="27" spans="1:4">
-      <x:c r="C27" s="3" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D27" s="0" t="s">
+      <x:c r="C25" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>250</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="C26" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4">
+      <x:c r="B28" s="1" t="s">
+        <x:v>251</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="B29" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C29" s="2" t="s">
+        <x:v>252</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4"/>
+    <x:row r="31" spans="1:4">
+      <x:c r="C31" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>253</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="C32" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>254</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4">
+      <x:c r="C33" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
         <x:v>249</x:v>
       </x:c>
     </x:row>
-    <x:row r="28" spans="1:4">
-      <x:c r="C28" s="3" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D28" s="0" t="s">
-        <x:v>250</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:4">
-      <x:c r="C29" s="3" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="D29" s="0" t="s">
-        <x:v>170</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:4">
-      <x:c r="B31" s="1" t="s">
-        <x:v>251</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:4">
-      <x:c r="B32" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C32" s="2" t="s">
-        <x:v>252</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:4"/>
     <x:row r="34" spans="1:4">
       <x:c r="C34" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D34" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:4">
       <x:c r="C35" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D35" s="0" t="s">
-        <x:v>254</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:4">
-      <x:c r="C36" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D36" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:4">
+      <x:c r="B37" s="1" t="s">
+        <x:v>256</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:4">
+      <x:c r="B38" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C38" s="2" t="s">
+        <x:v>257</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:4"/>
+    <x:row r="40" spans="1:4">
+      <x:c r="C40" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>253</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:4">
+      <x:c r="C41" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:4">
+      <x:c r="C42" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
         <x:v>249</x:v>
       </x:c>
     </x:row>
-    <x:row r="37" spans="1:4">
-      <x:c r="C37" s="3" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D37" s="0" t="s">
-        <x:v>255</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38" spans="1:4">
-      <x:c r="C38" s="3" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="D38" s="0" t="s">
-        <x:v>170</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40" spans="1:4">
-      <x:c r="B40" s="1" t="s">
-        <x:v>256</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="1:4">
-      <x:c r="B41" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C41" s="2" t="s">
-        <x:v>257</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="42" spans="1:4"/>
     <x:row r="43" spans="1:4">
       <x:c r="C43" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D43" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:4">
       <x:c r="C44" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D44" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="45" spans="1:4">
-      <x:c r="C45" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D45" s="0" t="s">
-        <x:v>249</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:4">
-      <x:c r="C46" s="3" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D46" s="0" t="s">
-        <x:v>255</x:v>
+      <x:c r="B46" s="1" t="s">
+        <x:v>258</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:4">
-      <x:c r="C47" s="3" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="D47" s="0" t="s">
-        <x:v>170</x:v>
-      </x:c>
-    </x:row>
+      <x:c r="B47" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C47" s="2" t="s">
+        <x:v>259</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:4"/>
     <x:row r="49" spans="1:4">
-      <x:c r="B49" s="1" t="s">
-        <x:v>258</x:v>
+      <x:c r="C49" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>253</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:4">
-      <x:c r="B50" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C50" s="2" t="s">
-        <x:v>259</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="51" spans="1:4"/>
+      <x:c r="C50" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:4">
+      <x:c r="C51" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+    </x:row>
     <x:row r="52" spans="1:4">
       <x:c r="C52" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D52" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:4">
       <x:c r="C53" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D53" s="0" t="s">
-        <x:v>260</x:v>
+        <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:4">
       <x:c r="C54" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D54" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:4">
+      <x:c r="B56" s="1" t="s">
+        <x:v>262</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:4">
+      <x:c r="B57" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C57" s="2" t="s">
+        <x:v>259</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:4"/>
+    <x:row r="59" spans="1:4">
+      <x:c r="C59" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D59" s="0" t="s">
+        <x:v>253</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:4">
+      <x:c r="C60" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D60" s="0" t="s">
+        <x:v>263</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:4">
+      <x:c r="C61" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D61" s="0" t="s">
         <x:v>261</x:v>
       </x:c>
     </x:row>
-    <x:row r="55" spans="1:4">
-      <x:c r="C55" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D55" s="0" t="s">
-        <x:v>249</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="56" spans="1:4">
-      <x:c r="C56" s="3" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D56" s="0" t="s">
-        <x:v>255</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="57" spans="1:4">
-      <x:c r="C57" s="3" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="D57" s="0" t="s">
-        <x:v>170</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="59" spans="1:4">
-      <x:c r="B59" s="1" t="s">
-        <x:v>262</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="60" spans="1:4">
-      <x:c r="B60" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C60" s="2" t="s">
-        <x:v>259</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="61" spans="1:4"/>
     <x:row r="62" spans="1:4">
       <x:c r="C62" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D62" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>264</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:4">
@@ -4648,7 +4666,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D63" s="0" t="s">
-        <x:v>263</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:4">
@@ -4656,46 +4674,22 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D64" s="0" t="s">
-        <x:v>261</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:4">
       <x:c r="C65" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D65" s="0" t="s">
-        <x:v>264</x:v>
+        <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:4">
       <x:c r="C66" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D66" s="0" t="s">
-        <x:v>76</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="67" spans="1:4">
-      <x:c r="C67" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D67" s="0" t="s">
-        <x:v>249</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="68" spans="1:4">
-      <x:c r="C68" s="3" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D68" s="0" t="s">
-        <x:v>255</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="69" spans="1:4">
-      <x:c r="C69" s="3" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="D69" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
     </x:row>

</xml_diff>